<commit_message>
Add VLANs and equipment
</commit_message>
<xml_diff>
--- a/Calculations.xlsx
+++ b/Calculations.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Proiecte\Facultate\AN_4\Sem2\CNDP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EDBB290-FB27-449C-8C3B-0D86044EB1CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9F65C2A-F1DF-4252-9A64-C8C71D7AAD2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cable calculations" sheetId="1" r:id="rId1"/>
+    <sheet name="VLANs" sheetId="2" r:id="rId2"/>
+    <sheet name="Equipment" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="169">
   <si>
     <t>Double outlets</t>
   </si>
@@ -105,27 +107,12 @@
     <t>IDF3</t>
   </si>
   <si>
-    <t>(IDF3) / MDF</t>
-  </si>
-  <si>
-    <t>(IDF1) / MDF</t>
-  </si>
-  <si>
-    <t>(IDF2) / IDF1</t>
-  </si>
-  <si>
     <t>IDF4</t>
   </si>
   <si>
     <t>IDF5</t>
   </si>
   <si>
-    <t>(IDF4)/IDF1</t>
-  </si>
-  <si>
-    <t>(IDF5)/IDF2</t>
-  </si>
-  <si>
     <t>Rooms per DF</t>
   </si>
   <si>
@@ -166,13 +153,397 @@
   </si>
   <si>
     <t>Average per outlet</t>
+  </si>
+  <si>
+    <t>(IDF2)</t>
+  </si>
+  <si>
+    <t>(IDF1)</t>
+  </si>
+  <si>
+    <t>(IDF3)</t>
+  </si>
+  <si>
+    <t>(IDF4)</t>
+  </si>
+  <si>
+    <t>(IDF5)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No. </t>
+  </si>
+  <si>
+    <t>VLAN NAME</t>
+  </si>
+  <si>
+    <t>DEFAULT GATEWAY</t>
+  </si>
+  <si>
+    <t>192.168.10.x</t>
+  </si>
+  <si>
+    <t>192.168.10.1</t>
+  </si>
+  <si>
+    <t>192.168.20.x</t>
+  </si>
+  <si>
+    <t>192.168.20.1</t>
+  </si>
+  <si>
+    <t>192.168.30.x</t>
+  </si>
+  <si>
+    <t>192.168.30.1</t>
+  </si>
+  <si>
+    <t>WLAN1</t>
+  </si>
+  <si>
+    <t>192.168.40.x</t>
+  </si>
+  <si>
+    <t>192.168.40.1</t>
+  </si>
+  <si>
+    <t>WLAN2</t>
+  </si>
+  <si>
+    <t>192.168.50.x</t>
+  </si>
+  <si>
+    <t>192.168.50.1</t>
+  </si>
+  <si>
+    <t>WLAN3</t>
+  </si>
+  <si>
+    <t>192.168.60.x</t>
+  </si>
+  <si>
+    <t>192.168.60.1</t>
+  </si>
+  <si>
+    <t>WLAN4</t>
+  </si>
+  <si>
+    <t>192.168.70.x</t>
+  </si>
+  <si>
+    <t>192.168.70.1</t>
+  </si>
+  <si>
+    <t>WLAN5</t>
+  </si>
+  <si>
+    <t>192.168.80.x</t>
+  </si>
+  <si>
+    <t>192.168.80.1</t>
+  </si>
+  <si>
+    <t>192.168.90.x</t>
+  </si>
+  <si>
+    <t>192.168.90.1</t>
+  </si>
+  <si>
+    <t>192.168.100.x</t>
+  </si>
+  <si>
+    <t>192.168.100.1</t>
+  </si>
+  <si>
+    <t>192.168.110.x</t>
+  </si>
+  <si>
+    <t>192.168.110.1</t>
+  </si>
+  <si>
+    <t>192.168.120.x</t>
+  </si>
+  <si>
+    <t>192.168.120.1</t>
+  </si>
+  <si>
+    <t>192.168.130.x</t>
+  </si>
+  <si>
+    <t>192.168.130.1</t>
+  </si>
+  <si>
+    <t>192.168.140.x</t>
+  </si>
+  <si>
+    <t>192.168.140.1</t>
+  </si>
+  <si>
+    <t>192.168.150.x</t>
+  </si>
+  <si>
+    <t>192.168.150.1</t>
+  </si>
+  <si>
+    <t>192.168.160.x</t>
+  </si>
+  <si>
+    <t>192.168.160.1</t>
+  </si>
+  <si>
+    <t>192.168.170.x</t>
+  </si>
+  <si>
+    <t>192.168.170.1</t>
+  </si>
+  <si>
+    <t>192.168.180.x</t>
+  </si>
+  <si>
+    <t>192.168.180.1</t>
+  </si>
+  <si>
+    <t>192.168.190.x</t>
+  </si>
+  <si>
+    <t>192.168.190.1</t>
+  </si>
+  <si>
+    <t>192.168.200.x</t>
+  </si>
+  <si>
+    <t>192.168.200.1</t>
+  </si>
+  <si>
+    <t>192.168.210.x</t>
+  </si>
+  <si>
+    <t>192.168.210.1</t>
+  </si>
+  <si>
+    <t>192.168.220.x</t>
+  </si>
+  <si>
+    <t>192.168.220.1</t>
+  </si>
+  <si>
+    <t>192.168.230.x</t>
+  </si>
+  <si>
+    <t>192.168.230.1</t>
+  </si>
+  <si>
+    <t>192.168.240.x</t>
+  </si>
+  <si>
+    <t>192.168.240.1</t>
+  </si>
+  <si>
+    <t>192.168.250.x</t>
+  </si>
+  <si>
+    <t>192.168.250.1</t>
+  </si>
+  <si>
+    <t>VLAN_MANAGEMENT</t>
+  </si>
+  <si>
+    <t>VOICE_VLAN</t>
+  </si>
+  <si>
+    <t>VOICE_VLAN2</t>
+  </si>
+  <si>
+    <t>VLAN_ALPHA</t>
+  </si>
+  <si>
+    <t>VLAN_BETA</t>
+  </si>
+  <si>
+    <t>VLAN_GAMMA</t>
+  </si>
+  <si>
+    <t>VLAN_DELTA</t>
+  </si>
+  <si>
+    <t>VLAN_EPSILON</t>
+  </si>
+  <si>
+    <t>VLAN_ZETA</t>
+  </si>
+  <si>
+    <t>VLAN_ETA</t>
+  </si>
+  <si>
+    <t>VLAN_THETA</t>
+  </si>
+  <si>
+    <t>VLAN_IOTA</t>
+  </si>
+  <si>
+    <t>VLAN_KAPPA</t>
+  </si>
+  <si>
+    <t>VLAN_LAMBDA</t>
+  </si>
+  <si>
+    <t>VLAN_MU</t>
+  </si>
+  <si>
+    <t>VLAN_NU</t>
+  </si>
+  <si>
+    <t>VLAN_XI</t>
+  </si>
+  <si>
+    <t>VLAN_OMICRON</t>
+  </si>
+  <si>
+    <t>VLAN_PI</t>
+  </si>
+  <si>
+    <t>VLAN_SIGMA</t>
+  </si>
+  <si>
+    <t>IP SUBNET /24</t>
+  </si>
+  <si>
+    <t>Firewall</t>
+  </si>
+  <si>
+    <t>Equipment name</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t>Details</t>
+  </si>
+  <si>
+    <t>&gt; at least 1310 ports</t>
+  </si>
+  <si>
+    <t>WLESS APs</t>
+  </si>
+  <si>
+    <t>Cisco C9600X-LC-56YL4C</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 56-port 50/25/10GE, 4-port 100GE Line Card</t>
+  </si>
+  <si>
+    <t>Juniper EX4650-48Y</t>
+  </si>
+  <si>
+    <t>$15,610.99</t>
+  </si>
+  <si>
+    <t>https://www.zones.com/site/product/index.html?id=106392241</t>
+  </si>
+  <si>
+    <t>https://www.tech-america.com/item/cisco-catalyst-9600-series-56-port-50g-4-port-100g/c9600x-lc-56yl4c</t>
+  </si>
+  <si>
+    <t>$25,698.00</t>
+  </si>
+  <si>
+    <t>Switch Layer 2/3 - modular</t>
+  </si>
+  <si>
+    <t>Cisco Firepower 9300 SM-56 x 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Palo Alto PA-7080 </t>
+  </si>
+  <si>
+    <t>590Gbps firewall throughput. *Results were derived from an optimum combination of PA-7000-DPC-A and PA-7000-100G-NPC-A cards populated in all available slots.</t>
+  </si>
+  <si>
+    <t>190gbps firewall throughput</t>
+  </si>
+  <si>
+    <t>https://www.zones.com/site/product/index.html?id=110211597</t>
+  </si>
+  <si>
+    <t>https://www.router-switch.com/paloalto-pan-pa-7080.html</t>
+  </si>
+  <si>
+    <t>https://itprice.com/paloalto/pan-pa-7000-100g-npc-a.html</t>
+  </si>
+  <si>
+    <t>https://www.zones.com/site/product/index.html?id=108729655</t>
+  </si>
+  <si>
+    <t>Cisco Catalyst CW9166D1-MR</t>
+  </si>
+  <si>
+    <t>https://www.cdw.com/product/cisco-catalyst-9166d1-wireless-access-point-bluetooth-wi-fi-6e-cloud/7569178</t>
+  </si>
+  <si>
+    <t>Ubiquiti U6 Enterprise</t>
+  </si>
+  <si>
+    <t>7.78 Gbps max throughput; 802.11ax support; Wi-fi6 - 6Hz; 1x 100M/1000M/2.5G/5G Multigigabit Ethernet; PoE</t>
+  </si>
+  <si>
+    <t>https://eu.store.ui.com/eu/en/collections/unifi-wifi-flagship-high-capacity/products/u6-enterprise</t>
+  </si>
+  <si>
+    <t>$280</t>
+  </si>
+  <si>
+    <t>$1,890</t>
+  </si>
+  <si>
+    <t>$535,000</t>
+  </si>
+  <si>
+    <t>$594,000</t>
+  </si>
+  <si>
+    <t>4.8 Gbps max throughput; 802.11ax support; Wi-fi6 - 6Hz; 1x 2.5 GbE; PoE; Works with software-based controller (UniFi Network Controller)</t>
+  </si>
+  <si>
+    <t>WLESS AP controllers</t>
+  </si>
+  <si>
+    <t>Ubiquiti Dream machine Special edition</t>
+  </si>
+  <si>
+    <t>$500</t>
+  </si>
+  <si>
+    <t>https://eu.store.ui.com/eu/en/collections/unifi-dream-machine</t>
+  </si>
+  <si>
+    <t>https://www.router-switch.com/c9800-80-k9.html</t>
+  </si>
+  <si>
+    <t>Cisco Catalyst 9800-80-k9</t>
+  </si>
+  <si>
+    <t>$30,000</t>
+  </si>
+  <si>
+    <t>Up to 6000 APs; up to 64k clients; 80 Gbps throughput; No support for Ubiquiti APs</t>
+  </si>
+  <si>
+    <t>1000+ PoE and PoE+; 3.5 Gbps routing; Includes full UniFi application suite for device management; 100+ UniFi devices; 1000+ client devices</t>
+  </si>
+  <si>
+    <t>48 x 1/10/25 Gigabit SFP28 + 8 x 40/100 Gigabit QSFP28 line card</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="168" formatCode="#,##0.00;[Red]#,##0.00"/>
+  </numFmts>
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -195,8 +566,53 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -215,8 +631,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -233,11 +655,64 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -246,14 +721,43 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -274,22 +778,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>2897605</xdr:colOff>
-      <xdr:row>108</xdr:row>
-      <xdr:rowOff>150396</xdr:rowOff>
+      <xdr:colOff>2898913</xdr:colOff>
+      <xdr:row>107</xdr:row>
+      <xdr:rowOff>157369</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>345406</xdr:colOff>
-      <xdr:row>134</xdr:row>
-      <xdr:rowOff>134855</xdr:rowOff>
+      <xdr:colOff>346213</xdr:colOff>
+      <xdr:row>133</xdr:row>
+      <xdr:rowOff>96492</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
+        <xdr:cNvPr id="6" name="Picture 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3E71DE26-1AE8-9014-731F-0A6B8BEE3919}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AA1358B0-DABE-D754-87D3-44ED53D0AE4F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -311,8 +815,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2897605" y="19691685"/>
-          <a:ext cx="7724775" cy="4676775"/>
+          <a:off x="2898913" y="19704326"/>
+          <a:ext cx="7734300" cy="4676775"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -589,8 +1093,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A103" zoomScale="86" zoomScaleNormal="67" workbookViewId="0">
-      <selection activeCell="L113" sqref="L113"/>
+    <sheetView topLeftCell="A69" zoomScale="75" zoomScaleNormal="67" workbookViewId="0">
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -609,19 +1113,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="6"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
+      <c r="A2" s="7"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -634,19 +1138,19 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
+      <c r="A7" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
       <c r="E7" s="5"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
@@ -654,12 +1158,12 @@
       <c r="C9" s="1"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
+      <c r="A10" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
@@ -677,10 +1181,10 @@
         <v>0</v>
       </c>
       <c r="E13" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="F13" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="G13" t="s">
         <v>4</v>
@@ -825,7 +1329,7 @@
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+      <c r="A18" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B18">
@@ -835,8 +1339,7 @@
         <v>42</v>
       </c>
       <c r="D18">
-        <f t="shared" si="0"/>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E18">
         <v>0</v>
@@ -850,11 +1353,11 @@
       </c>
       <c r="H18">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="I18">
         <f t="shared" si="3"/>
-        <v>180</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
@@ -1175,7 +1678,7 @@
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
+      <c r="A29" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B29">
@@ -1185,8 +1688,7 @@
         <v>42</v>
       </c>
       <c r="D29">
-        <f t="shared" si="0"/>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E29">
         <v>0</v>
@@ -1196,15 +1698,15 @@
         <v>12</v>
       </c>
       <c r="G29" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="H29">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="I29">
         <f t="shared" si="3"/>
-        <v>180</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
@@ -1660,7 +2162,7 @@
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
+      <c r="A44" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B44">
@@ -1670,8 +2172,7 @@
         <v>31</v>
       </c>
       <c r="D44">
-        <f t="shared" si="0"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E44">
         <v>0</v>
@@ -1681,15 +2182,15 @@
         <v>10</v>
       </c>
       <c r="G44" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="H44">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="I44">
         <f t="shared" si="3"/>
-        <v>128</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.3">
@@ -1858,7 +2359,7 @@
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A50" s="2" t="s">
+      <c r="A50" s="6" t="s">
         <v>25</v>
       </c>
       <c r="B50" s="2">
@@ -1868,8 +2369,7 @@
         <v>41</v>
       </c>
       <c r="D50" s="2">
-        <f t="shared" si="0"/>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E50" s="2">
         <v>0</v>
@@ -1879,15 +2379,15 @@
         <v>12</v>
       </c>
       <c r="G50" s="2" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="H50" s="2">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="I50" s="2">
         <f t="shared" si="3"/>
-        <v>180</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.3">
@@ -2142,7 +2642,7 @@
         <v>29</v>
       </c>
       <c r="G58" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="H58">
         <f t="shared" si="1"/>
@@ -2253,8 +2753,8 @@
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A62" t="s">
-        <v>29</v>
+      <c r="A62" s="3" t="s">
+        <v>26</v>
       </c>
       <c r="B62">
         <v>159</v>
@@ -2263,8 +2763,7 @@
         <v>31</v>
       </c>
       <c r="D62">
-        <f t="shared" si="0"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E62">
         <v>0</v>
@@ -2274,15 +2773,15 @@
         <v>10</v>
       </c>
       <c r="G62" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="H62">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="I62">
         <f t="shared" si="3"/>
-        <v>128</v>
+        <v>0</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.3">
@@ -2307,7 +2806,7 @@
         <v>13</v>
       </c>
       <c r="G63" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="H63">
         <f t="shared" si="1"/>
@@ -2340,7 +2839,7 @@
         <v>13</v>
       </c>
       <c r="G64" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="H64">
         <f t="shared" si="1"/>
@@ -2372,7 +2871,7 @@
         <v>12</v>
       </c>
       <c r="G65" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="H65">
         <f t="shared" si="1"/>
@@ -2438,7 +2937,7 @@
         <v>7</v>
       </c>
       <c r="G67" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="H67">
         <f t="shared" si="1"/>
@@ -2471,7 +2970,7 @@
         <v>19</v>
       </c>
       <c r="G68" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="H68">
         <f t="shared" si="1"/>
@@ -2561,7 +3060,7 @@
         <v>12</v>
       </c>
       <c r="G71" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="H71">
         <f t="shared" si="1"/>
@@ -2652,7 +3151,7 @@
         <v>8</v>
       </c>
       <c r="G74" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="H74">
         <f t="shared" si="1"/>
@@ -2685,7 +3184,7 @@
         <v>8</v>
       </c>
       <c r="G75" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="H75">
         <f t="shared" si="1"/>
@@ -2718,7 +3217,7 @@
         <v>7</v>
       </c>
       <c r="G76" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="H76">
         <f t="shared" si="1"/>
@@ -2751,7 +3250,7 @@
         <v>9</v>
       </c>
       <c r="G77" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="H77">
         <f t="shared" si="1"/>
@@ -2784,7 +3283,7 @@
         <v>29</v>
       </c>
       <c r="G78" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="H78">
         <f t="shared" si="1"/>
@@ -2797,7 +3296,7 @@
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B79">
         <v>176</v>
@@ -2817,7 +3316,7 @@
         <v>35</v>
       </c>
       <c r="G79" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="H79">
         <f t="shared" ref="H79:H88" si="5">D79*2</f>
@@ -2830,7 +3329,7 @@
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B80">
         <v>176</v>
@@ -2850,7 +3349,7 @@
         <v>35</v>
       </c>
       <c r="G80" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="H80">
         <f t="shared" si="5"/>
@@ -2882,7 +3381,7 @@
         <v>12</v>
       </c>
       <c r="G81" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="H81">
         <f t="shared" si="5"/>
@@ -2915,7 +3414,7 @@
         <v>13</v>
       </c>
       <c r="G82" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="H82">
         <f t="shared" si="5"/>
@@ -2948,7 +3447,7 @@
         <v>12</v>
       </c>
       <c r="G83" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="H83">
         <f t="shared" si="5"/>
@@ -2981,7 +3480,7 @@
         <v>13</v>
       </c>
       <c r="G84" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="H84">
         <f t="shared" si="5"/>
@@ -3014,7 +3513,7 @@
         <v>12</v>
       </c>
       <c r="G85" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="H85">
         <f t="shared" si="5"/>
@@ -3026,8 +3525,8 @@
       </c>
     </row>
     <row r="86" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A86" t="s">
-        <v>30</v>
+      <c r="A86" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B86">
         <v>182</v>
@@ -3036,8 +3535,7 @@
         <v>41</v>
       </c>
       <c r="D86">
-        <f t="shared" si="4"/>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E86">
         <v>0</v>
@@ -3047,20 +3545,20 @@
         <v>12</v>
       </c>
       <c r="G86" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="H86">
         <f t="shared" si="5"/>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="I86">
         <f t="shared" si="6"/>
-        <v>180</v>
+        <v>0</v>
       </c>
     </row>
     <row r="87" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B87">
         <v>184</v>
@@ -3080,7 +3578,7 @@
         <v>28</v>
       </c>
       <c r="G87" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="H87">
         <f t="shared" si="5"/>
@@ -3093,7 +3591,7 @@
     </row>
     <row r="88" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B88">
         <v>184</v>
@@ -3126,49 +3624,49 @@
     </row>
     <row r="90" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B90" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="D90">
         <f>SUM(D14:D88)</f>
-        <v>683</v>
+        <v>655</v>
       </c>
       <c r="H90" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="I90">
         <f>SUM(I14:I88)</f>
-        <v>60076</v>
+        <v>59100</v>
       </c>
       <c r="K90" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="L90">
         <f>ROUNDUP(I90/ (2 *D90), 0)</f>
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="91" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B91" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="D91">
         <f>2*D90</f>
-        <v>1366</v>
+        <v>1310</v>
       </c>
       <c r="H91" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="I91">
         <f>ROUNDUP(I90/305 + ROUNDUP(I90/305,0) * 10%, 0)</f>
-        <v>217</v>
+        <v>214</v>
       </c>
     </row>
     <row r="96" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B96" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="E96" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="97" spans="2:6" x14ac:dyDescent="0.3">
@@ -3237,14 +3735,14 @@
     </row>
     <row r="101" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B101" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C101">
         <f>COUNTIF(G14:G88, "IDF4")</f>
         <v>10</v>
       </c>
       <c r="E101" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="F101">
         <f>SUMIFS($D$14:$D$88, $G$14:$G$88, "IDF4")</f>
@@ -3253,14 +3751,14 @@
     </row>
     <row r="102" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B102" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C102">
         <f>COUNTIF(G14:G88, "IDF5")</f>
         <v>10</v>
       </c>
       <c r="E102" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F102">
         <f>SUMIFS($D$14:$D$88, $G$14:$G$88, "IDF5")</f>
@@ -3269,13 +3767,13 @@
     </row>
     <row r="106" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B106" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="107" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B107">
-        <f>(5+27 + 35 + 111 + 5 +27+78+108)+6*12</f>
-        <v>468</v>
+        <f>(5*2+27 + 32 + 113 + 5+27*3+78*2+108)+6*16</f>
+        <v>628</v>
       </c>
     </row>
   </sheetData>
@@ -3290,4 +3788,719 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA837CA2-3D9E-4EB2-AF47-6C89AB1F7D60}">
+  <dimension ref="A1:D26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="21.88671875" customWidth="1"/>
+    <col min="3" max="3" width="20" customWidth="1"/>
+    <col min="4" max="4" width="20.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="11">
+        <v>1</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="9">
+        <f>A2+1</f>
+        <v>2</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="9">
+        <f t="shared" ref="A4:A26" si="0">A3+1</f>
+        <v>3</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="9">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="9">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="9">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="9">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="9">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="9">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="9">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="9">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="9">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="9">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="9">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="9">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="9">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="9">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="9">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="9">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="9">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="D21" s="10" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="9">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="9">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="9">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="9">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="9">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>104</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6F91D44-F9DE-40FC-932A-19DA19B4DB91}">
+  <dimension ref="A1:Q27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="94" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="35" style="15" customWidth="1"/>
+    <col min="2" max="2" width="11.109375" style="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.21875" style="15" customWidth="1"/>
+    <col min="4" max="4" width="46.77734375" style="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.88671875" style="15"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="15">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="15">
+        <f>2*C1</f>
+        <v>1310</v>
+      </c>
+      <c r="D2" s="15" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="14" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="16" t="s">
+        <v>133</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>139</v>
+      </c>
+      <c r="C9" s="19" t="s">
+        <v>138</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="15" t="s">
+        <v>135</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="C10" s="19" t="s">
+        <v>137</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="14" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="17" t="s">
+        <v>149</v>
+      </c>
+      <c r="B14" s="18" t="s">
+        <v>155</v>
+      </c>
+      <c r="C14" s="19" t="s">
+        <v>150</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="16" t="s">
+        <v>151</v>
+      </c>
+      <c r="B15" s="18" t="s">
+        <v>154</v>
+      </c>
+      <c r="C15" s="19" t="s">
+        <v>153</v>
+      </c>
+      <c r="D15" s="15" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="23"/>
+      <c r="B16" s="18"/>
+      <c r="C16" s="19"/>
+    </row>
+    <row r="17" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A17" s="14" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A18" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="D18" s="13" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A19" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="B19" s="18" t="s">
+        <v>165</v>
+      </c>
+      <c r="C19" s="19" t="s">
+        <v>163</v>
+      </c>
+      <c r="D19" s="15" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A20" s="16" t="s">
+        <v>160</v>
+      </c>
+      <c r="B20" s="18" t="s">
+        <v>161</v>
+      </c>
+      <c r="C20" s="19" t="s">
+        <v>162</v>
+      </c>
+      <c r="D20" s="15" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A22" s="14" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A23" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="B23" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="C23" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="D23" s="13" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A24" s="15" t="s">
+        <v>141</v>
+      </c>
+      <c r="B24" s="20" t="s">
+        <v>156</v>
+      </c>
+      <c r="C24" s="19" t="s">
+        <v>145</v>
+      </c>
+      <c r="D24" s="21" t="s">
+        <v>144</v>
+      </c>
+      <c r="E24" s="21"/>
+      <c r="F24" s="21"/>
+      <c r="G24" s="21"/>
+      <c r="H24" s="21"/>
+      <c r="I24" s="21"/>
+      <c r="J24" s="21"/>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A25" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="B25" s="20" t="s">
+        <v>157</v>
+      </c>
+      <c r="C25" s="19" t="s">
+        <v>146</v>
+      </c>
+      <c r="D25" s="22" t="s">
+        <v>143</v>
+      </c>
+      <c r="E25" s="22"/>
+      <c r="F25" s="22"/>
+      <c r="G25" s="22"/>
+      <c r="H25" s="22"/>
+      <c r="I25" s="22"/>
+      <c r="J25" s="22"/>
+      <c r="K25" s="22"/>
+      <c r="L25" s="22"/>
+      <c r="M25" s="22"/>
+      <c r="N25" s="22"/>
+      <c r="O25" s="21"/>
+      <c r="P25" s="21"/>
+      <c r="Q25" s="21"/>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="C26" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="D26" s="22"/>
+      <c r="E26" s="22"/>
+      <c r="F26" s="22"/>
+      <c r="G26" s="22"/>
+      <c r="H26" s="22"/>
+      <c r="I26" s="22"/>
+      <c r="J26" s="22"/>
+      <c r="K26" s="22"/>
+      <c r="L26" s="22"/>
+      <c r="M26" s="22"/>
+      <c r="N26" s="22"/>
+      <c r="O26" s="21"/>
+      <c r="P26" s="21"/>
+      <c r="Q26" s="21"/>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="C27" s="19" t="s">
+        <v>148</v>
+      </c>
+      <c r="D27" s="22"/>
+      <c r="E27" s="22"/>
+      <c r="F27" s="22"/>
+      <c r="G27" s="22"/>
+      <c r="H27" s="22"/>
+      <c r="I27" s="22"/>
+      <c r="J27" s="22"/>
+      <c r="K27" s="22"/>
+      <c r="L27" s="22"/>
+      <c r="M27" s="22"/>
+      <c r="N27" s="22"/>
+      <c r="O27" s="21"/>
+      <c r="P27" s="21"/>
+      <c r="Q27" s="21"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="D25:N27"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="C14" r:id="rId1" xr:uid="{2C0E2546-2E3A-4840-91C6-9F130E685735}"/>
+    <hyperlink ref="C15" r:id="rId2" xr:uid="{55CFC80E-4AC6-40FB-8984-283B86BF1D6E}"/>
+    <hyperlink ref="C9" r:id="rId3" xr:uid="{4F395D3C-B6C9-422F-A4F6-BBDE9F92D8D4}"/>
+    <hyperlink ref="C10" r:id="rId4" xr:uid="{04EBA3C9-9BB2-48EA-B7FA-5A470E553A89}"/>
+    <hyperlink ref="C24" r:id="rId5" xr:uid="{1940ACB3-3B2F-46E4-9068-31F6BA2FDEE5}"/>
+    <hyperlink ref="C25" r:id="rId6" xr:uid="{E463D737-C232-45F9-A0CF-532B40A0B53F}"/>
+    <hyperlink ref="C26" r:id="rId7" xr:uid="{57F7B904-3E48-423B-802C-83BD2ABD15EC}"/>
+    <hyperlink ref="C27" r:id="rId8" xr:uid="{61F9F295-0985-42BB-912E-BDA0C470ACEB}"/>
+    <hyperlink ref="C19" r:id="rId9" xr:uid="{ECCD9621-B9CB-42F8-9CB5-9F8DEF0879E3}"/>
+    <hyperlink ref="C20" r:id="rId10" xr:uid="{833F4F48-2814-4D15-AED1-A96BC35D176E}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add Rack model and equipment data sheet links
</commit_message>
<xml_diff>
--- a/Calculations.xlsx
+++ b/Calculations.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Proiecte\Facultate\AN_4\Sem2\CNDP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9F65C2A-F1DF-4252-9A64-C8C71D7AAD2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98BC4F3E-3A2D-4145-B7FF-14ECC156424C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="167">
   <si>
     <t>Double outlets</t>
   </si>
@@ -74,9 +74,6 @@
     <t>Bathroom</t>
   </si>
   <si>
-    <t>IDF</t>
-  </si>
-  <si>
     <t>Storage</t>
   </si>
   <si>
@@ -431,27 +428,15 @@
     <t>Cisco C9600X-LC-56YL4C</t>
   </si>
   <si>
-    <t xml:space="preserve"> 56-port 50/25/10GE, 4-port 100GE Line Card</t>
-  </si>
-  <si>
     <t>Juniper EX4650-48Y</t>
   </si>
   <si>
     <t>$15,610.99</t>
   </si>
   <si>
-    <t>https://www.zones.com/site/product/index.html?id=106392241</t>
-  </si>
-  <si>
-    <t>https://www.tech-america.com/item/cisco-catalyst-9600-series-56-port-50g-4-port-100g/c9600x-lc-56yl4c</t>
-  </si>
-  <si>
     <t>$25,698.00</t>
   </si>
   <si>
-    <t>Switch Layer 2/3 - modular</t>
-  </si>
-  <si>
     <t>Cisco Firepower 9300 SM-56 x 3</t>
   </si>
   <si>
@@ -464,33 +449,15 @@
     <t>190gbps firewall throughput</t>
   </si>
   <si>
-    <t>https://www.zones.com/site/product/index.html?id=110211597</t>
-  </si>
-  <si>
-    <t>https://www.router-switch.com/paloalto-pan-pa-7080.html</t>
-  </si>
-  <si>
-    <t>https://itprice.com/paloalto/pan-pa-7000-100g-npc-a.html</t>
-  </si>
-  <si>
-    <t>https://www.zones.com/site/product/index.html?id=108729655</t>
-  </si>
-  <si>
     <t>Cisco Catalyst CW9166D1-MR</t>
   </si>
   <si>
-    <t>https://www.cdw.com/product/cisco-catalyst-9166d1-wireless-access-point-bluetooth-wi-fi-6e-cloud/7569178</t>
-  </si>
-  <si>
     <t>Ubiquiti U6 Enterprise</t>
   </si>
   <si>
     <t>7.78 Gbps max throughput; 802.11ax support; Wi-fi6 - 6Hz; 1x 100M/1000M/2.5G/5G Multigigabit Ethernet; PoE</t>
   </si>
   <si>
-    <t>https://eu.store.ui.com/eu/en/collections/unifi-wifi-flagship-high-capacity/products/u6-enterprise</t>
-  </si>
-  <si>
     <t>$280</t>
   </si>
   <si>
@@ -515,12 +482,6 @@
     <t>$500</t>
   </si>
   <si>
-    <t>https://eu.store.ui.com/eu/en/collections/unifi-dream-machine</t>
-  </si>
-  <si>
-    <t>https://www.router-switch.com/c9800-80-k9.html</t>
-  </si>
-  <si>
     <t>Cisco Catalyst 9800-80-k9</t>
   </si>
   <si>
@@ -533,7 +494,40 @@
     <t>1000+ PoE and PoE+; 3.5 Gbps routing; Includes full UniFi application suite for device management; 100+ UniFi devices; 1000+ client devices</t>
   </si>
   <si>
-    <t>48 x 1/10/25 Gigabit SFP28 + 8 x 40/100 Gigabit QSFP28 line card</t>
+    <t>Supervisor</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 56-port 50/25/10GE, 4-port 100GE Line Card; fiber optic support</t>
+  </si>
+  <si>
+    <t>48 x 1/10/25 Gigabit SFP28 + 8 x 40/100 Gigabit QSFP28 line card; fiber optic support</t>
+  </si>
+  <si>
+    <t>Switch Layer 2/3 + FO - modular</t>
+  </si>
+  <si>
+    <t>https://www.cisco.com/c/en/us/products/collateral/switches/catalyst-9600-series-switches/nb-06-cat9600-series-line-data-sheet-cte-en.html</t>
+  </si>
+  <si>
+    <t>https://www.juniper.net/content/dam/www/assets/datasheets/us/en/switches/ex4650-ethernet-switch-datasheet.pdf</t>
+  </si>
+  <si>
+    <t>https://www.cisco.com/c/en/us/products/collateral/wireless/catalyst-9166-series-access-points/catalyst-9166-series-access-points-ds.html</t>
+  </si>
+  <si>
+    <t>https://dl.ui.com/ds/u6-enterprise_ds.pdf</t>
+  </si>
+  <si>
+    <t>https://www.cisco.com/c/en/us/products/collateral/wireless/catalyst-9800-series-wireless-controllers/nb-06-cat9800-80-wirel-mod-data-sheet-ctp-en.html</t>
+  </si>
+  <si>
+    <t>https://dl.ui.com/ds/udm_se_ds.pdf</t>
+  </si>
+  <si>
+    <t>https://www.cisco.com/c/en/us/products/collateral/security/firepower-9000-series/datasheet-c78-742471.html</t>
+  </si>
+  <si>
+    <t>https://www.paloaltonetworks.com/resources/datasheets/pa-7000-series</t>
   </si>
 </sst>
 </file>
@@ -541,7 +535,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="#,##0.00;[Red]#,##0.00"/>
+    <numFmt numFmtId="164" formatCode="#,##0.00;[Red]#,##0.00"/>
   </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
@@ -712,7 +706,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -722,12 +716,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
@@ -742,19 +730,24 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1093,8 +1086,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L107"/>
   <sheetViews>
-    <sheetView topLeftCell="A69" zoomScale="75" zoomScaleNormal="67" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+    <sheetView topLeftCell="A86" zoomScale="106" zoomScaleNormal="67" workbookViewId="0">
+      <selection activeCell="G94" sqref="G94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1113,44 +1106,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="7"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
+      <c r="A2" s="18"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" s="18"/>
+      <c r="C7" s="18"/>
+      <c r="E7" s="5"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="18" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="E7" s="5"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
+      <c r="B8" s="18"/>
+      <c r="C8" s="18"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
@@ -1158,12 +1151,12 @@
       <c r="C9" s="1"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
+      <c r="A10" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="18"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
@@ -1181,10 +1174,10 @@
         <v>0</v>
       </c>
       <c r="E13" t="s">
+        <v>32</v>
+      </c>
+      <c r="F13" t="s">
         <v>33</v>
-      </c>
-      <c r="F13" t="s">
-        <v>34</v>
       </c>
       <c r="G13" t="s">
         <v>4</v>
@@ -1349,7 +1342,7 @@
         <v>12</v>
       </c>
       <c r="G18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H18">
         <f t="shared" si="1"/>
@@ -1546,7 +1539,7 @@
         <v>12</v>
       </c>
       <c r="G24" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H24">
         <f t="shared" si="1"/>
@@ -1666,7 +1659,7 @@
         <v>47</v>
       </c>
       <c r="G28" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H28">
         <f t="shared" si="1"/>
@@ -1679,7 +1672,7 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B29">
         <v>123</v>
@@ -1698,7 +1691,7 @@
         <v>12</v>
       </c>
       <c r="G29" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H29">
         <f t="shared" si="1"/>
@@ -1731,7 +1724,7 @@
         <v>13</v>
       </c>
       <c r="G30" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H30">
         <f t="shared" si="1"/>
@@ -1764,7 +1757,7 @@
         <v>12</v>
       </c>
       <c r="G31" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H31">
         <f t="shared" si="1"/>
@@ -1797,7 +1790,7 @@
         <v>13</v>
       </c>
       <c r="G32" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H32">
         <f t="shared" si="1"/>
@@ -1829,7 +1822,7 @@
         <v>12</v>
       </c>
       <c r="G33" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H33">
         <f t="shared" si="1"/>
@@ -1862,7 +1855,7 @@
         <v>24</v>
       </c>
       <c r="G34" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H34">
         <f t="shared" si="1"/>
@@ -1895,7 +1888,7 @@
         <v>28</v>
       </c>
       <c r="G35" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H35">
         <f t="shared" si="1"/>
@@ -1908,7 +1901,7 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B36">
         <v>131</v>
@@ -1928,7 +1921,7 @@
         <v>9</v>
       </c>
       <c r="G36" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H36">
         <f t="shared" si="1"/>
@@ -1961,7 +1954,7 @@
         <v>8</v>
       </c>
       <c r="G37" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H37">
         <f t="shared" si="1"/>
@@ -1994,7 +1987,7 @@
         <v>8</v>
       </c>
       <c r="G38" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H38">
         <f t="shared" si="1"/>
@@ -2027,7 +2020,7 @@
         <v>8</v>
       </c>
       <c r="G39" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H39">
         <f t="shared" si="1"/>
@@ -2059,7 +2052,7 @@
         <v>12</v>
       </c>
       <c r="G40" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H40">
         <f t="shared" si="1"/>
@@ -2130,7 +2123,7 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B43">
         <v>139</v>
@@ -2150,7 +2143,7 @@
         <v>19</v>
       </c>
       <c r="G43" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H43">
         <f t="shared" si="1"/>
@@ -2163,7 +2156,7 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B44">
         <v>140</v>
@@ -2182,7 +2175,7 @@
         <v>10</v>
       </c>
       <c r="G44" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H44">
         <f t="shared" si="1"/>
@@ -2215,7 +2208,7 @@
         <v>25</v>
       </c>
       <c r="G45" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H45">
         <f t="shared" si="1"/>
@@ -2228,7 +2221,7 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B46">
         <v>142</v>
@@ -2248,7 +2241,7 @@
         <v>13</v>
       </c>
       <c r="G46" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H46">
         <f t="shared" si="1"/>
@@ -2261,7 +2254,7 @@
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B47">
         <v>143</v>
@@ -2281,7 +2274,7 @@
         <v>13</v>
       </c>
       <c r="G47" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H47">
         <f t="shared" si="1"/>
@@ -2294,7 +2287,7 @@
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B48">
         <v>144</v>
@@ -2314,7 +2307,7 @@
         <v>13</v>
       </c>
       <c r="G48" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H48">
         <f t="shared" si="1"/>
@@ -2347,7 +2340,7 @@
         <v>8</v>
       </c>
       <c r="G49" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H49">
         <f t="shared" si="1"/>
@@ -2360,7 +2353,7 @@
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B50" s="2">
         <v>147</v>
@@ -2379,7 +2372,7 @@
         <v>12</v>
       </c>
       <c r="G50" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H50" s="2">
         <f t="shared" si="1"/>
@@ -2412,7 +2405,7 @@
         <v>12</v>
       </c>
       <c r="G51" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H51">
         <f t="shared" si="1"/>
@@ -2445,7 +2438,7 @@
         <v>13</v>
       </c>
       <c r="G52" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H52">
         <f t="shared" si="1"/>
@@ -2478,7 +2471,7 @@
         <v>12</v>
       </c>
       <c r="G53" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H53">
         <f t="shared" si="1"/>
@@ -2511,7 +2504,7 @@
         <v>13</v>
       </c>
       <c r="G54" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H54">
         <f t="shared" si="1"/>
@@ -2543,7 +2536,7 @@
         <v>12</v>
       </c>
       <c r="G55" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H55">
         <f t="shared" si="1"/>
@@ -2576,7 +2569,7 @@
         <v>43</v>
       </c>
       <c r="G56" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H56">
         <f t="shared" si="1"/>
@@ -2609,7 +2602,7 @@
         <v>27</v>
       </c>
       <c r="G57" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H57">
         <f t="shared" si="1"/>
@@ -2642,7 +2635,7 @@
         <v>29</v>
       </c>
       <c r="G58" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H58">
         <f t="shared" si="1"/>
@@ -2675,7 +2668,7 @@
         <v>8</v>
       </c>
       <c r="G59" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H59">
         <f t="shared" si="1"/>
@@ -2708,7 +2701,7 @@
         <v>8</v>
       </c>
       <c r="G60" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H60">
         <f t="shared" si="1"/>
@@ -2721,7 +2714,7 @@
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B61">
         <v>158</v>
@@ -2741,7 +2734,7 @@
         <v>13</v>
       </c>
       <c r="G61" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H61">
         <f t="shared" si="1"/>
@@ -2754,7 +2747,7 @@
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A62" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B62">
         <v>159</v>
@@ -2773,7 +2766,7 @@
         <v>10</v>
       </c>
       <c r="G62" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H62">
         <f t="shared" si="1"/>
@@ -2786,7 +2779,7 @@
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B63">
         <v>160</v>
@@ -2806,7 +2799,7 @@
         <v>13</v>
       </c>
       <c r="G63" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H63">
         <f t="shared" si="1"/>
@@ -2819,7 +2812,7 @@
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B64">
         <v>161</v>
@@ -2839,7 +2832,7 @@
         <v>13</v>
       </c>
       <c r="G64" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H64">
         <f t="shared" si="1"/>
@@ -2871,7 +2864,7 @@
         <v>12</v>
       </c>
       <c r="G65" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H65">
         <f t="shared" si="1"/>
@@ -2904,7 +2897,7 @@
         <v>17</v>
       </c>
       <c r="G66" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H66">
         <f t="shared" si="1"/>
@@ -2917,7 +2910,7 @@
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B67">
         <v>164</v>
@@ -2937,7 +2930,7 @@
         <v>7</v>
       </c>
       <c r="G67" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H67">
         <f t="shared" si="1"/>
@@ -2950,7 +2943,7 @@
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B68">
         <v>165</v>
@@ -2970,7 +2963,7 @@
         <v>19</v>
       </c>
       <c r="G68" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H68">
         <f t="shared" si="1"/>
@@ -3060,7 +3053,7 @@
         <v>12</v>
       </c>
       <c r="G71" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H71">
         <f t="shared" si="1"/>
@@ -3151,7 +3144,7 @@
         <v>8</v>
       </c>
       <c r="G74" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H74">
         <f t="shared" si="1"/>
@@ -3184,7 +3177,7 @@
         <v>8</v>
       </c>
       <c r="G75" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H75">
         <f t="shared" si="1"/>
@@ -3217,7 +3210,7 @@
         <v>7</v>
       </c>
       <c r="G76" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H76">
         <f t="shared" si="1"/>
@@ -3230,7 +3223,7 @@
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B77">
         <v>174</v>
@@ -3250,7 +3243,7 @@
         <v>9</v>
       </c>
       <c r="G77" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H77">
         <f t="shared" si="1"/>
@@ -3283,7 +3276,7 @@
         <v>29</v>
       </c>
       <c r="G78" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H78">
         <f t="shared" si="1"/>
@@ -3296,7 +3289,7 @@
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B79">
         <v>176</v>
@@ -3316,7 +3309,7 @@
         <v>35</v>
       </c>
       <c r="G79" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H79">
         <f t="shared" ref="H79:H88" si="5">D79*2</f>
@@ -3329,7 +3322,7 @@
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B80">
         <v>176</v>
@@ -3349,7 +3342,7 @@
         <v>35</v>
       </c>
       <c r="G80" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H80">
         <f t="shared" si="5"/>
@@ -3381,7 +3374,7 @@
         <v>12</v>
       </c>
       <c r="G81" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H81">
         <f t="shared" si="5"/>
@@ -3414,7 +3407,7 @@
         <v>13</v>
       </c>
       <c r="G82" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H82">
         <f t="shared" si="5"/>
@@ -3447,7 +3440,7 @@
         <v>12</v>
       </c>
       <c r="G83" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H83">
         <f t="shared" si="5"/>
@@ -3480,7 +3473,7 @@
         <v>13</v>
       </c>
       <c r="G84" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H84">
         <f t="shared" si="5"/>
@@ -3513,7 +3506,7 @@
         <v>12</v>
       </c>
       <c r="G85" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H85">
         <f t="shared" si="5"/>
@@ -3526,7 +3519,7 @@
     </row>
     <row r="86" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A86" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B86">
         <v>182</v>
@@ -3545,7 +3538,7 @@
         <v>12</v>
       </c>
       <c r="G86" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H86">
         <f t="shared" si="5"/>
@@ -3558,7 +3551,7 @@
     </row>
     <row r="87" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B87">
         <v>184</v>
@@ -3578,7 +3571,7 @@
         <v>28</v>
       </c>
       <c r="G87" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H87">
         <f t="shared" si="5"/>
@@ -3591,7 +3584,7 @@
     </row>
     <row r="88" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B88">
         <v>184</v>
@@ -3611,7 +3604,7 @@
         <v>28</v>
       </c>
       <c r="G88" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="H88">
         <f t="shared" si="5"/>
@@ -3624,21 +3617,21 @@
     </row>
     <row r="90" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B90" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D90">
         <f>SUM(D14:D88)</f>
         <v>655</v>
       </c>
       <c r="H90" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I90">
         <f>SUM(I14:I88)</f>
         <v>59100</v>
       </c>
       <c r="K90" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L90">
         <f>ROUNDUP(I90/ (2 *D90), 0)</f>
@@ -3647,14 +3640,14 @@
     </row>
     <row r="91" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B91" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D91">
         <f>2*D90</f>
         <v>1310</v>
       </c>
       <c r="H91" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I91">
         <f>ROUNDUP(I90/305 + ROUNDUP(I90/305,0) * 10%, 0)</f>
@@ -3663,10 +3656,10 @@
     </row>
     <row r="96" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B96" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E96" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="97" spans="2:6" x14ac:dyDescent="0.3">
@@ -3687,14 +3680,14 @@
     </row>
     <row r="98" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B98" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C98">
         <f>COUNTIF(G14:G88, "IDF1")</f>
         <v>11</v>
       </c>
       <c r="E98" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F98">
         <f>SUMIFS($D$14:$D$88, $G$14:$G$88, "IDF1")</f>
@@ -3703,14 +3696,14 @@
     </row>
     <row r="99" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B99" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C99">
         <f>COUNTIF(G14:G88, "IDF2")</f>
         <v>8</v>
       </c>
       <c r="E99" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F99">
         <f>SUMIFS($D$14:$D$88, $G$14:$G$88, "IDF2")</f>
@@ -3719,14 +3712,14 @@
     </row>
     <row r="100" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B100" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C100">
         <f>COUNTIF(G14:G88, "IDF3")</f>
         <v>11</v>
       </c>
       <c r="E100" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F100">
         <f>SUMIFS($D$14:$D$88, $G$14:$G$88, "IDF3")</f>
@@ -3735,14 +3728,14 @@
     </row>
     <row r="101" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B101" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C101">
         <f>COUNTIF(G14:G88, "IDF4")</f>
         <v>10</v>
       </c>
       <c r="E101" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F101">
         <f>SUMIFS($D$14:$D$88, $G$14:$G$88, "IDF4")</f>
@@ -3751,23 +3744,23 @@
     </row>
     <row r="102" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B102" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C102">
         <f>COUNTIF(G14:G88, "IDF5")</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E102" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F102">
         <f>SUMIFS($D$14:$D$88, $G$14:$G$88, "IDF5")</f>
-        <v>96</v>
+        <v>121</v>
       </c>
     </row>
     <row r="106" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B106" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="107" spans="2:6" x14ac:dyDescent="0.3">
@@ -3806,391 +3799,391 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="C1" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="D1" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="C1" s="13" t="s">
-        <v>125</v>
-      </c>
-      <c r="D1" s="13" t="s">
+    </row>
+    <row r="2" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="9">
+        <v>1</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="C2" s="10" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="11">
-        <v>1</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>105</v>
-      </c>
-      <c r="C2" s="12" t="s">
+      <c r="D2" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="D2" s="12" t="s">
-        <v>51</v>
-      </c>
     </row>
     <row r="3" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="9">
+      <c r="A3" s="7">
         <f>A2+1</f>
         <v>2</v>
       </c>
-      <c r="B3" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="C3" s="10" t="s">
+      <c r="B3" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="D3" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="D3" s="10" t="s">
-        <v>53</v>
-      </c>
     </row>
     <row r="4" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="9">
+      <c r="A4" s="7">
         <f t="shared" ref="A4:A26" si="0">A3+1</f>
         <v>3</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="7">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="7">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="7">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="7">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="7">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="7">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B10" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="C4" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="9">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="9">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="9">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="9">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="9">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="B9" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="D9" s="10" t="s">
+      <c r="C10" s="8" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="9">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="B10" s="10" t="s">
+      <c r="D10" s="8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="7">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B11" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="C10" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="D10" s="10" t="s">
+      <c r="C11" s="8" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="9">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="B11" s="10" t="s">
+      <c r="D11" s="8" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="7">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="B12" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="C11" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="D11" s="10" t="s">
+      <c r="C12" s="8" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="9">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="B12" s="10" t="s">
+      <c r="D12" s="8" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="7">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="B13" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="C12" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="D12" s="10" t="s">
+      <c r="C13" s="8" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="9">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="B13" s="10" t="s">
+      <c r="D13" s="8" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="7">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="B14" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="C13" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="D13" s="10" t="s">
+      <c r="C14" s="8" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="9">
-        <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
-      <c r="B14" s="10" t="s">
+      <c r="D14" s="8" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="7">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="B15" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="C14" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="D14" s="10" t="s">
+      <c r="C15" s="8" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="9">
-        <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-      <c r="B15" s="10" t="s">
+      <c r="D15" s="8" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="7">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="B16" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="C15" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="D15" s="10" t="s">
+      <c r="C16" s="8" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="9">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="B16" s="10" t="s">
+      <c r="D16" s="8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="7">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="B17" s="8" t="s">
         <v>114</v>
       </c>
-      <c r="C16" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="D16" s="10" t="s">
+      <c r="C17" s="8" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="9">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="B17" s="10" t="s">
+      <c r="D17" s="8" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="7">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="B18" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="C17" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="D17" s="10" t="s">
+      <c r="C18" s="8" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="9">
-        <f t="shared" si="0"/>
-        <v>17</v>
-      </c>
-      <c r="B18" s="10" t="s">
+      <c r="D18" s="8" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="7">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="B19" s="8" t="s">
         <v>116</v>
       </c>
-      <c r="C18" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="D18" s="10" t="s">
+      <c r="C19" s="8" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="9">
-        <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
-      <c r="B19" s="10" t="s">
+      <c r="D19" s="8" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="7">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="B20" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="C19" s="10" t="s">
-        <v>89</v>
-      </c>
-      <c r="D19" s="10" t="s">
+      <c r="C20" s="8" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="9">
-        <f t="shared" si="0"/>
-        <v>19</v>
-      </c>
-      <c r="B20" s="10" t="s">
+      <c r="D20" s="8" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="7">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="B21" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="C20" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="D20" s="10" t="s">
+      <c r="C21" s="8" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="9">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="B21" s="10" t="s">
+      <c r="D21" s="8" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="7">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="B22" s="8" t="s">
         <v>119</v>
       </c>
-      <c r="C21" s="10" t="s">
-        <v>93</v>
-      </c>
-      <c r="D21" s="10" t="s">
+      <c r="C22" s="8" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="9">
-        <f t="shared" si="0"/>
-        <v>21</v>
-      </c>
-      <c r="B22" s="10" t="s">
+      <c r="D22" s="8" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="7">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="B23" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="C22" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="D22" s="10" t="s">
+      <c r="C23" s="8" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="9">
-        <f t="shared" si="0"/>
-        <v>22</v>
-      </c>
-      <c r="B23" s="10" t="s">
+      <c r="D23" s="8" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="7">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="B24" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="C23" s="10" t="s">
-        <v>97</v>
-      </c>
-      <c r="D23" s="10" t="s">
+      <c r="C24" s="8" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="9">
-        <f t="shared" si="0"/>
-        <v>23</v>
-      </c>
-      <c r="B24" s="10" t="s">
+      <c r="D24" s="8" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="7">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="B25" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="C24" s="10" t="s">
-        <v>99</v>
-      </c>
-      <c r="D24" s="10" t="s">
+      <c r="C25" s="8" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="9">
-        <f t="shared" si="0"/>
-        <v>24</v>
-      </c>
-      <c r="B25" s="10" t="s">
+      <c r="D25" s="8" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="7">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="B26" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="C25" s="10" t="s">
-        <v>101</v>
-      </c>
-      <c r="D25" s="10" t="s">
+      <c r="C26" s="8" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="9">
-        <f t="shared" si="0"/>
-        <v>25</v>
-      </c>
-      <c r="B26" s="10" t="s">
-        <v>124</v>
-      </c>
-      <c r="C26" s="10" t="s">
+      <c r="D26" s="8" t="s">
         <v>103</v>
-      </c>
-      <c r="D26" s="10" t="s">
-        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -4200,257 +4193,253 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6F91D44-F9DE-40FC-932A-19DA19B4DB91}">
-  <dimension ref="A1:Q27"/>
+  <dimension ref="A1:Q32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="94" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="98" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35" style="15" customWidth="1"/>
-    <col min="2" max="2" width="11.109375" style="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.21875" style="15" customWidth="1"/>
-    <col min="4" max="4" width="46.77734375" style="15" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.88671875" style="15"/>
+    <col min="1" max="1" width="35" customWidth="1"/>
+    <col min="2" max="2" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.21875" customWidth="1"/>
+    <col min="4" max="4" width="46.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="C1" s="15">
+      <c r="A1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1">
         <v>655</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="C2" s="15">
+      <c r="A2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2">
         <f>2*C1</f>
         <v>1310</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="D2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="12" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="B9" t="s">
+        <v>135</v>
+      </c>
+      <c r="C9" s="21" t="s">
+        <v>159</v>
+      </c>
+      <c r="D9" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>133</v>
+      </c>
+      <c r="B10" t="s">
+        <v>134</v>
+      </c>
+      <c r="C10" s="21" t="s">
+        <v>160</v>
+      </c>
+      <c r="D10" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="12" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="14" t="s">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="14" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="13" t="s">
+      <c r="B14" s="15" t="s">
+        <v>144</v>
+      </c>
+      <c r="C14" s="21" t="s">
+        <v>161</v>
+      </c>
+      <c r="D14" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>143</v>
+      </c>
+      <c r="C15" s="21" t="s">
+        <v>162</v>
+      </c>
+      <c r="D15" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B16" s="15"/>
+      <c r="C16" s="16"/>
+    </row>
+    <row r="17" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A17" s="12" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A18" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="B18" s="11" t="s">
         <v>127</v>
       </c>
-      <c r="B8" s="13" t="s">
+      <c r="C18" s="11" t="s">
         <v>128</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="D18" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="D8" s="13" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="16" t="s">
-        <v>133</v>
-      </c>
-      <c r="B9" s="15" t="s">
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A19" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="B19" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="C19" s="21" t="s">
+        <v>163</v>
+      </c>
+      <c r="D19" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A20" s="13" t="s">
+        <v>149</v>
+      </c>
+      <c r="B20" s="15" t="s">
+        <v>150</v>
+      </c>
+      <c r="C20" s="21" t="s">
+        <v>164</v>
+      </c>
+      <c r="D20" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A22" s="12" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A23" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="D23" s="11" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>136</v>
+      </c>
+      <c r="B24" s="17" t="s">
+        <v>145</v>
+      </c>
+      <c r="C24" s="21" t="s">
+        <v>165</v>
+      </c>
+      <c r="D24" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="C9" s="19" t="s">
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+    </row>
+    <row r="25" spans="1:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="B25" s="17" t="s">
+        <v>146</v>
+      </c>
+      <c r="C25" s="21" t="s">
+        <v>166</v>
+      </c>
+      <c r="D25" s="20" t="s">
         <v>138</v>
       </c>
-      <c r="D9" s="15" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="15" t="s">
-        <v>135</v>
-      </c>
-      <c r="B10" s="15" t="s">
-        <v>136</v>
-      </c>
-      <c r="C10" s="19" t="s">
-        <v>137</v>
-      </c>
-      <c r="D10" s="15" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A12" s="14" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="B13" s="13" t="s">
-        <v>128</v>
-      </c>
-      <c r="C13" s="13" t="s">
-        <v>129</v>
-      </c>
-      <c r="D13" s="13" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="17" t="s">
-        <v>149</v>
-      </c>
-      <c r="B14" s="18" t="s">
-        <v>155</v>
-      </c>
-      <c r="C14" s="19" t="s">
-        <v>150</v>
-      </c>
-      <c r="D14" s="15" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="16" t="s">
-        <v>151</v>
-      </c>
-      <c r="B15" s="18" t="s">
-        <v>154</v>
-      </c>
-      <c r="C15" s="19" t="s">
-        <v>153</v>
-      </c>
-      <c r="D15" s="15" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="23"/>
-      <c r="B16" s="18"/>
-      <c r="C16" s="19"/>
-    </row>
-    <row r="17" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A17" s="14" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A18" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="B18" s="13" t="s">
-        <v>128</v>
-      </c>
-      <c r="C18" s="13" t="s">
-        <v>129</v>
-      </c>
-      <c r="D18" s="13" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A19" s="17" t="s">
-        <v>164</v>
-      </c>
-      <c r="B19" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="C19" s="19" t="s">
-        <v>163</v>
-      </c>
-      <c r="D19" s="15" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A20" s="16" t="s">
-        <v>160</v>
-      </c>
-      <c r="B20" s="18" t="s">
-        <v>161</v>
-      </c>
-      <c r="C20" s="19" t="s">
-        <v>162</v>
-      </c>
-      <c r="D20" s="15" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A22" s="14" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A23" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="B23" s="13" t="s">
-        <v>128</v>
-      </c>
-      <c r="C23" s="13" t="s">
-        <v>129</v>
-      </c>
-      <c r="D23" s="13" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A24" s="15" t="s">
-        <v>141</v>
-      </c>
-      <c r="B24" s="20" t="s">
-        <v>156</v>
-      </c>
-      <c r="C24" s="19" t="s">
-        <v>145</v>
-      </c>
-      <c r="D24" s="21" t="s">
-        <v>144</v>
-      </c>
-      <c r="E24" s="21"/>
-      <c r="F24" s="21"/>
-      <c r="G24" s="21"/>
-      <c r="H24" s="21"/>
-      <c r="I24" s="21"/>
-      <c r="J24" s="21"/>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A25" s="16" t="s">
-        <v>142</v>
-      </c>
-      <c r="B25" s="20" t="s">
-        <v>157</v>
-      </c>
-      <c r="C25" s="19" t="s">
-        <v>146</v>
-      </c>
-      <c r="D25" s="22" t="s">
-        <v>143</v>
-      </c>
-      <c r="E25" s="22"/>
-      <c r="F25" s="22"/>
-      <c r="G25" s="22"/>
-      <c r="H25" s="22"/>
-      <c r="I25" s="22"/>
-      <c r="J25" s="22"/>
-      <c r="K25" s="22"/>
-      <c r="L25" s="22"/>
-      <c r="M25" s="22"/>
-      <c r="N25" s="22"/>
-      <c r="O25" s="21"/>
-      <c r="P25" s="21"/>
-      <c r="Q25" s="21"/>
+      <c r="E25" s="20"/>
+      <c r="F25" s="20"/>
+      <c r="G25" s="20"/>
+      <c r="H25" s="20"/>
+      <c r="I25" s="20"/>
+      <c r="J25" s="20"/>
+      <c r="K25" s="20"/>
+      <c r="L25" s="20"/>
+      <c r="M25" s="20"/>
+      <c r="N25" s="20"/>
+      <c r="O25" s="20"/>
+      <c r="P25" s="1"/>
+      <c r="Q25" s="1"/>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="C26" s="19" t="s">
-        <v>147</v>
-      </c>
+      <c r="C26" s="16"/>
       <c r="D26" s="22"/>
       <c r="E26" s="22"/>
       <c r="F26" s="22"/>
@@ -4462,14 +4451,12 @@
       <c r="L26" s="22"/>
       <c r="M26" s="22"/>
       <c r="N26" s="22"/>
-      <c r="O26" s="21"/>
-      <c r="P26" s="21"/>
-      <c r="Q26" s="21"/>
+      <c r="O26" s="1"/>
+      <c r="P26" s="1"/>
+      <c r="Q26" s="1"/>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="C27" s="19" t="s">
-        <v>148</v>
-      </c>
+      <c r="C27" s="16"/>
       <c r="D27" s="22"/>
       <c r="E27" s="22"/>
       <c r="F27" s="22"/>
@@ -4481,13 +4468,42 @@
       <c r="L27" s="22"/>
       <c r="M27" s="22"/>
       <c r="N27" s="22"/>
-      <c r="O27" s="21"/>
-      <c r="P27" s="21"/>
-      <c r="Q27" s="21"/>
+      <c r="O27" s="1"/>
+      <c r="P27" s="1"/>
+      <c r="Q27" s="1"/>
+    </row>
+    <row r="28" spans="1:17" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="29" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A29" s="12" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A30" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="B30" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="C30" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="D30" s="11" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A31" s="14"/>
+      <c r="B31" s="15"/>
+      <c r="C31" s="16"/>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B32" s="15"/>
+      <c r="C32" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="D25:N27"/>
+    <mergeCell ref="D25:O25"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C14" r:id="rId1" xr:uid="{2C0E2546-2E3A-4840-91C6-9F130E685735}"/>
@@ -4496,10 +4512,8 @@
     <hyperlink ref="C10" r:id="rId4" xr:uid="{04EBA3C9-9BB2-48EA-B7FA-5A470E553A89}"/>
     <hyperlink ref="C24" r:id="rId5" xr:uid="{1940ACB3-3B2F-46E4-9068-31F6BA2FDEE5}"/>
     <hyperlink ref="C25" r:id="rId6" xr:uid="{E463D737-C232-45F9-A0CF-532B40A0B53F}"/>
-    <hyperlink ref="C26" r:id="rId7" xr:uid="{57F7B904-3E48-423B-802C-83BD2ABD15EC}"/>
-    <hyperlink ref="C27" r:id="rId8" xr:uid="{61F9F295-0985-42BB-912E-BDA0C470ACEB}"/>
-    <hyperlink ref="C19" r:id="rId9" xr:uid="{ECCD9621-B9CB-42F8-9CB5-9F8DEF0879E3}"/>
-    <hyperlink ref="C20" r:id="rId10" xr:uid="{833F4F48-2814-4D15-AED1-A96BC35D176E}"/>
+    <hyperlink ref="C19" r:id="rId7" xr:uid="{ECCD9621-B9CB-42F8-9CB5-9F8DEF0879E3}"/>
+    <hyperlink ref="C20" r:id="rId8" xr:uid="{833F4F48-2814-4D15-AED1-A96BC35D176E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>